<commit_message>
Auo Refresh. Only show IPOST PDFs Issues: SRC not refereshing, Error when no pdfs in source folder
</commit_message>
<xml_diff>
--- a/TS Post Database Inserter/Resources/SourceExcel.xlsx
+++ b/TS Post Database Inserter/Resources/SourceExcel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\lol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talle\source\repos\TS Post Database Inserter\TS Post Database Inserter\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A2107669-BF30-4A19-A37B-DADE7AE07A1B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -54,12 +55,18 @@
   </si>
   <si>
     <t>ParcelNumber</t>
+  </si>
+  <si>
+    <t>ParcelSize</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,11 +411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="A2:J8"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,9 +430,11 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,6 +464,12 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>